<commit_message>
scrape players that script missed and added validation to ensure all players were scraped
</commit_message>
<xml_diff>
--- a/PlayerToPro/data/pro_season_data.xlsx
+++ b/PlayerToPro/data/pro_season_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caleb/Desktop/Waterloo/IST/PlayerToPro/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741396F4-D079-3A4D-92E5-299F8E45F4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069CD609-ADB1-A548-88F9-1AD4848F6688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15098" uniqueCount="2969">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15508" uniqueCount="3036">
   <si>
     <t>Player</t>
   </si>
@@ -8927,13 +8927,214 @@
   </si>
   <si>
     <t>Detroit Pistons</t>
+  </si>
+  <si>
+    <t>Sami Al Uariachi</t>
+  </si>
+  <si>
+    <t>Damex UDEA Algeciras</t>
+  </si>
+  <si>
+    <t>Adil El Makssoud</t>
+  </si>
+  <si>
+    <t>Fath US de Rabat</t>
+  </si>
+  <si>
+    <t>Chabab Rif Al Hoceima</t>
+  </si>
+  <si>
+    <t>Kevin Leander Fiabema</t>
+  </si>
+  <si>
+    <t>Oppsal Tigers</t>
+  </si>
+  <si>
+    <t>Atanas (Nasko) Golomeev</t>
+  </si>
+  <si>
+    <t>PBC Academic Sofia</t>
+  </si>
+  <si>
+    <t>1971-72</t>
+  </si>
+  <si>
+    <t>1972-73</t>
+  </si>
+  <si>
+    <t>BC Levski Sofia</t>
+  </si>
+  <si>
+    <t>Adana Demirspor</t>
+  </si>
+  <si>
+    <t>Daniel Gonzalez Longarela</t>
+  </si>
+  <si>
+    <t>Marc Antoine Horth</t>
+  </si>
+  <si>
+    <t>Misi Boye Jeanneau-Mubiala</t>
+  </si>
+  <si>
+    <t>Michael Kelvin II</t>
+  </si>
+  <si>
+    <t>Radhi Knapp</t>
+  </si>
+  <si>
+    <t>Franck Olivier Kouagnia</t>
+  </si>
+  <si>
+    <t>Eskilstuna Basket</t>
+  </si>
+  <si>
+    <t>Wetterbygden Stars Huskvarna</t>
+  </si>
+  <si>
+    <t>Fundacion Globalcaja La Roda</t>
+  </si>
+  <si>
+    <t>Sorgues BC</t>
+  </si>
+  <si>
+    <t>Islam Luiz de Toledo</t>
+  </si>
+  <si>
+    <t>Carioca</t>
+  </si>
+  <si>
+    <t>Ginastico B.Horizont</t>
+  </si>
+  <si>
+    <t>A.B.A. Araraquara</t>
+  </si>
+  <si>
+    <t>David John Oates</t>
+  </si>
+  <si>
+    <t>Darwin Eagles</t>
+  </si>
+  <si>
+    <t>Rotimi Osuntola Jr.</t>
+  </si>
+  <si>
+    <t>CP Agustinos-Eras E. Leclerc Leon</t>
+  </si>
+  <si>
+    <t>Jean Emmanuel Pierre-Charles</t>
+  </si>
+  <si>
+    <t>San Luis Santos Reales</t>
+  </si>
+  <si>
+    <t>Santos de San Luis Potosi</t>
+  </si>
+  <si>
+    <t>Alejandro Prescott-Cornejo</t>
+  </si>
+  <si>
+    <t>CB Andujar Jean Paraiso Interi</t>
+  </si>
+  <si>
+    <t>N'Kosi Kedar Salam</t>
+  </si>
+  <si>
+    <t>Tobarra CB</t>
+  </si>
+  <si>
+    <t>City of Badajoz Academy</t>
+  </si>
+  <si>
+    <t>Ismar Serferagic Kriese</t>
+  </si>
+  <si>
+    <t>MTV Wolfenbuettel von 2012 Herzoege</t>
+  </si>
+  <si>
+    <t>VfL Stade</t>
+  </si>
+  <si>
+    <t>Weser Baskets Bremen/BTS Neustadt</t>
+  </si>
+  <si>
+    <t>Bremen 1860</t>
+  </si>
+  <si>
+    <t>Rob Smart Jr.</t>
+  </si>
+  <si>
+    <t>Kevin St. Kitts</t>
+  </si>
+  <si>
+    <t>Earl Thompson Jr.</t>
+  </si>
+  <si>
+    <t>Team Solent Kestrels 2nd team</t>
+  </si>
+  <si>
+    <t>S.C. Rarense</t>
+  </si>
+  <si>
+    <t>Henry Van Herk</t>
+  </si>
+  <si>
+    <t>Iserlohn Kangaroos</t>
+  </si>
+  <si>
+    <t>BG 2000 Berlin</t>
+  </si>
+  <si>
+    <t>Bas van Willigen</t>
+  </si>
+  <si>
+    <t>Haaglanden Cobra's Voorburg</t>
+  </si>
+  <si>
+    <t>Eiffel Towers Nijmegen</t>
+  </si>
+  <si>
+    <t>Fun 4 All Bergen-Op-Zoom</t>
+  </si>
+  <si>
+    <t>Myleasecar.nl</t>
+  </si>
+  <si>
+    <t>Tulip Den Bosch</t>
+  </si>
+  <si>
+    <t>PromotieDivisie</t>
+  </si>
+  <si>
+    <t>VBC Akrides</t>
+  </si>
+  <si>
+    <t>Samuel Willis III</t>
+  </si>
+  <si>
+    <t>Gloria</t>
+  </si>
+  <si>
+    <t>Luka Zaharijevic</t>
+  </si>
+  <si>
+    <t>Palangos Kursiai</t>
+  </si>
+  <si>
+    <t>Hita Plasticos CBA</t>
+  </si>
+  <si>
+    <t>Jason Scully</t>
+  </si>
+  <si>
+    <t>Ryan Smith</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8946,6 +9147,25 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -8983,11 +9203,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9290,10 +9516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3088"/>
+  <dimension ref="A1:E3178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A3164" workbookViewId="0">
+      <selection activeCell="C3181" sqref="C3181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -60771,6 +60997,1472 @@
         <v>2968</v>
       </c>
     </row>
+    <row r="3089" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3089" s="2" t="s">
+        <v>2969</v>
+      </c>
+      <c r="B3089" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3089" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3089" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3089" s="2" t="s">
+        <v>2970</v>
+      </c>
+    </row>
+    <row r="3090" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3090" s="2" t="s">
+        <v>2971</v>
+      </c>
+      <c r="B3090" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3090" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3090" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3090" s="5" t="s">
+        <v>2972</v>
+      </c>
+    </row>
+    <row r="3091" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3091" s="2" t="s">
+        <v>2971</v>
+      </c>
+      <c r="B3091" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="C3091" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3091" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3091" s="5" t="s">
+        <v>2973</v>
+      </c>
+    </row>
+    <row r="3092" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3092" s="2" t="s">
+        <v>2974</v>
+      </c>
+      <c r="B3092" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3092" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D3092" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="E3092" s="5" t="s">
+        <v>2975</v>
+      </c>
+    </row>
+    <row r="3093" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3093" s="2" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B3093" s="4" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C3093" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D3093" s="5"/>
+      <c r="E3093" s="5" t="s">
+        <v>2977</v>
+      </c>
+    </row>
+    <row r="3094" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3094" s="2" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B3094" s="4" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C3094" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D3094" s="5"/>
+      <c r="E3094" s="5" t="s">
+        <v>2977</v>
+      </c>
+    </row>
+    <row r="3095" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3095" s="2" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B3095" s="4" t="s">
+        <v>2978</v>
+      </c>
+      <c r="C3095" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D3095" s="5"/>
+      <c r="E3095" s="5" t="s">
+        <v>2977</v>
+      </c>
+    </row>
+    <row r="3096" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3096" s="2" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B3096" s="4" t="s">
+        <v>2979</v>
+      </c>
+      <c r="C3096" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D3096" s="5"/>
+      <c r="E3096" s="5" t="s">
+        <v>2977</v>
+      </c>
+    </row>
+    <row r="3097" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3097" s="2" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B3097" s="4" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C3097" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D3097" s="5"/>
+      <c r="E3097" s="5" t="s">
+        <v>2977</v>
+      </c>
+    </row>
+    <row r="3098" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3098" s="2" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B3098" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="C3098" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D3098" s="5"/>
+      <c r="E3098" s="5" t="s">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="3099" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3099" s="2" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B3099" s="4" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C3099" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D3099" s="5"/>
+      <c r="E3099" s="5" t="s">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="3100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3100" s="2" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B3100" s="4" t="s">
+        <v>741</v>
+      </c>
+      <c r="C3100" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D3100" s="5"/>
+      <c r="E3100" s="5" t="s">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="3101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3101" s="2" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B3101" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="C3101" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D3101" s="5"/>
+      <c r="E3101" s="5" t="s">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="3102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3102" s="2" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B3102" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C3102" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D3102" s="5"/>
+      <c r="E3102" s="5" t="s">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="3103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3103" s="2" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B3103" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C3103" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D3103" s="5"/>
+      <c r="E3103" s="5" t="s">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="3104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3104" s="2" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B3104" s="4" t="s">
+        <v>925</v>
+      </c>
+      <c r="C3104" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D3104" s="5"/>
+      <c r="E3104" s="5" t="s">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="3105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3105" s="2" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B3105" s="4" t="s">
+        <v>929</v>
+      </c>
+      <c r="C3105" s="5" t="s">
+        <v>732</v>
+      </c>
+      <c r="D3105" s="5"/>
+      <c r="E3105" s="5" t="s">
+        <v>2981</v>
+      </c>
+    </row>
+    <row r="3106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3106" s="2" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B3106" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="C3106" s="5" t="s">
+        <v>732</v>
+      </c>
+      <c r="D3106" s="5"/>
+      <c r="E3106" s="5" t="s">
+        <v>2981</v>
+      </c>
+    </row>
+    <row r="3107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3107" s="2" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B3107" s="4" t="s">
+        <v>931</v>
+      </c>
+      <c r="C3107" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D3107" s="5"/>
+      <c r="E3107" s="5" t="s">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="3108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3108" s="2" t="s">
+        <v>2982</v>
+      </c>
+      <c r="B3108" s="4">
+        <v>2023</v>
+      </c>
+      <c r="C3108" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3108" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3108" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3109" s="2" t="s">
+        <v>2983</v>
+      </c>
+      <c r="B3109" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="C3109" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3109" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3109" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3110" s="2" t="s">
+        <v>2983</v>
+      </c>
+      <c r="B3110" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3110" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3110" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3110" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3111" s="2" t="s">
+        <v>2984</v>
+      </c>
+      <c r="B3111" s="4">
+        <v>2023</v>
+      </c>
+      <c r="C3111" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3111" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3111" s="5" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="3112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3112" s="2" t="s">
+        <v>2985</v>
+      </c>
+      <c r="B3112" s="4">
+        <v>2024</v>
+      </c>
+      <c r="C3112" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3112" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3112" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3113" s="2" t="s">
+        <v>2986</v>
+      </c>
+      <c r="B3113" s="4">
+        <v>2004</v>
+      </c>
+      <c r="C3113" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3113" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E3113" s="5" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="3114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3114" s="2" t="s">
+        <v>2986</v>
+      </c>
+      <c r="B3114" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3114" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3114" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3114" s="5" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="3115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3115" s="2" t="s">
+        <v>2986</v>
+      </c>
+      <c r="B3115" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3115" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3115" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3115" s="5" t="s">
+        <v>2653</v>
+      </c>
+    </row>
+    <row r="3116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3116" s="2" t="s">
+        <v>2986</v>
+      </c>
+      <c r="B3116" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="C3116" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3116" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3116" s="5" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="3117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3117" s="2" t="s">
+        <v>2987</v>
+      </c>
+      <c r="B3117" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="C3117" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D3117" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="E3117" s="5" t="s">
+        <v>2988</v>
+      </c>
+    </row>
+    <row r="3118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3118" s="2" t="s">
+        <v>2987</v>
+      </c>
+      <c r="B3118" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3118" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D3118" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3118" s="5" t="s">
+        <v>2989</v>
+      </c>
+    </row>
+    <row r="3119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3119" s="2" t="s">
+        <v>2987</v>
+      </c>
+      <c r="B3119" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3119" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3119" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3119" s="5" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="3120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3120" s="2" t="s">
+        <v>2987</v>
+      </c>
+      <c r="B3120" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3120" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3120" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3120" s="5" t="s">
+        <v>2990</v>
+      </c>
+    </row>
+    <row r="3121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3121" s="2" t="s">
+        <v>2987</v>
+      </c>
+      <c r="B3121" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3121" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3121" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="E3121" s="5" t="s">
+        <v>2991</v>
+      </c>
+    </row>
+    <row r="3122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3122" s="2" t="s">
+        <v>2992</v>
+      </c>
+      <c r="B3122" s="4">
+        <v>2013</v>
+      </c>
+      <c r="C3122" s="5" t="s">
+        <v>853</v>
+      </c>
+      <c r="D3122" s="5" t="s">
+        <v>2993</v>
+      </c>
+      <c r="E3122" s="5" t="s">
+        <v>2994</v>
+      </c>
+    </row>
+    <row r="3123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3123" s="2" t="s">
+        <v>2992</v>
+      </c>
+      <c r="B3123" s="4">
+        <v>2017</v>
+      </c>
+      <c r="C3123" s="5" t="s">
+        <v>853</v>
+      </c>
+      <c r="D3123" s="5" t="s">
+        <v>854</v>
+      </c>
+      <c r="E3123" s="5" t="s">
+        <v>2995</v>
+      </c>
+    </row>
+    <row r="3124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3124" s="2" t="s">
+        <v>2996</v>
+      </c>
+      <c r="B3124" s="4">
+        <v>2019</v>
+      </c>
+      <c r="C3124" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3124" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="E3124" s="5" t="s">
+        <v>2997</v>
+      </c>
+    </row>
+    <row r="3125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3125" s="2" t="s">
+        <v>2998</v>
+      </c>
+      <c r="B3125" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3125" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3125" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3125" s="5" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="3126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3126" s="2" t="s">
+        <v>2998</v>
+      </c>
+      <c r="B3126" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3126" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3126" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3126" s="5" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="3127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3127" s="2" t="s">
+        <v>3000</v>
+      </c>
+      <c r="B3127" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3127" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3127" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3127" s="5" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="3128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3128" s="2" t="s">
+        <v>3000</v>
+      </c>
+      <c r="B3128" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3128" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3128" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3128" s="5" t="s">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="3129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3129" s="2" t="s">
+        <v>3000</v>
+      </c>
+      <c r="B3129" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3129" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3129" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3129" s="5" t="s">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="3130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3130" s="2" t="s">
+        <v>3000</v>
+      </c>
+      <c r="B3130" s="4">
+        <v>2020</v>
+      </c>
+      <c r="C3130" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3130" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3130" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3131" s="2" t="s">
+        <v>3003</v>
+      </c>
+      <c r="B3131" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3131" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3131" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3131" s="5" t="s">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="3132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3132" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="B3132" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3132" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3132" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3132" s="5" t="s">
+        <v>2835</v>
+      </c>
+    </row>
+    <row r="3133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3133" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="B3133" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3133" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3133" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3133" s="5" t="s">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="3134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3134" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="B3134" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3134" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3134" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3134" s="5" t="s">
+        <v>2173</v>
+      </c>
+    </row>
+    <row r="3135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3135" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="B3135" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3135" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3135" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3135" s="5" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="3136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3136" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="B3136" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3136" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3136" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3136" s="5" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="3137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3137" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="B3137" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3137" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3137" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3137" s="5" t="s">
+        <v>2945</v>
+      </c>
+    </row>
+    <row r="3138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3138" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="B3138" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3138" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3138" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3138" s="5" t="s">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="3139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3139" s="2" t="s">
+        <v>3005</v>
+      </c>
+      <c r="B3139" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3139" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3139" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3139" s="5" t="s">
+        <v>2990</v>
+      </c>
+    </row>
+    <row r="3140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3140" s="2" t="s">
+        <v>3008</v>
+      </c>
+      <c r="B3140" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3140" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3140" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="E3140" s="5" t="s">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="3141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3141" s="2" t="s">
+        <v>3008</v>
+      </c>
+      <c r="B3141" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3141" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3141" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="E3141" s="5" t="s">
+        <v>3010</v>
+      </c>
+    </row>
+    <row r="3142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3142" s="2" t="s">
+        <v>3008</v>
+      </c>
+      <c r="B3142" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3142" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3142" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="E3142" s="5" t="s">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="3143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3143" s="2" t="s">
+        <v>3008</v>
+      </c>
+      <c r="B3143" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3143" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3143" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="E3143" s="5" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="3144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3144" s="2" t="s">
+        <v>3008</v>
+      </c>
+      <c r="B3144" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3144" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3144" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3144" s="5" t="s">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="3145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3145" s="2" t="s">
+        <v>3013</v>
+      </c>
+      <c r="B3145" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C3145" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3145" s="5" t="s">
+        <v>667</v>
+      </c>
+      <c r="E3145" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3146" s="2" t="s">
+        <v>3014</v>
+      </c>
+      <c r="B3146" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3146" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3146" s="5"/>
+      <c r="E3146" s="5" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="3147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3147" s="2" t="s">
+        <v>3014</v>
+      </c>
+      <c r="B3147" s="4" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C3147" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3147" s="5"/>
+      <c r="E3147" s="5" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="3148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3148" s="2" t="s">
+        <v>3014</v>
+      </c>
+      <c r="B3148" s="4" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C3148" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3148" s="5"/>
+      <c r="E3148" s="5" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="3149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3149" s="2" t="s">
+        <v>3014</v>
+      </c>
+      <c r="B3149" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="C3149" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3149" s="5"/>
+      <c r="E3149" s="5" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="3150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3150" s="2" t="s">
+        <v>3014</v>
+      </c>
+      <c r="B3150" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="C3150" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3150" s="5"/>
+      <c r="E3150" s="5" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="3151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3151" s="2" t="s">
+        <v>3014</v>
+      </c>
+      <c r="B3151" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="C3151" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3151" s="5"/>
+      <c r="E3151" s="5" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="3152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3152" s="2" t="s">
+        <v>3014</v>
+      </c>
+      <c r="B3152" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="C3152" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3152" s="5"/>
+      <c r="E3152" s="5" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="3153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3153" s="2" t="s">
+        <v>3014</v>
+      </c>
+      <c r="B3153" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="C3153" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3153" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="E3153" s="5" t="s">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="3154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3154" s="2" t="s">
+        <v>3014</v>
+      </c>
+      <c r="B3154" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3154" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3154" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3154" s="5" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="3155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3155" s="2" t="s">
+        <v>3014</v>
+      </c>
+      <c r="B3155" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3155" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3155" s="5"/>
+      <c r="E3155" s="5" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="3156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3156" s="2" t="s">
+        <v>3014</v>
+      </c>
+      <c r="B3156" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3156" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3156" s="5"/>
+      <c r="E3156" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3157" s="2" t="s">
+        <v>3014</v>
+      </c>
+      <c r="B3157" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="C3157" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3157" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3157" s="5" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="3158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3158" s="2" t="s">
+        <v>3015</v>
+      </c>
+      <c r="B3158" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3158" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3158" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3158" s="5" t="s">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="3159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3159" s="2" t="s">
+        <v>3015</v>
+      </c>
+      <c r="B3159" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3159" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D3159" s="5" t="s">
+        <v>674</v>
+      </c>
+      <c r="E3159" s="5" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="3160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3160" s="2" t="s">
+        <v>3018</v>
+      </c>
+      <c r="B3160" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3160" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3160" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="E3160" s="5" t="s">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="3161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3161" s="2" t="s">
+        <v>3018</v>
+      </c>
+      <c r="B3161" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3161" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3161" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3161" s="5" t="s">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="3162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3162" s="2" t="s">
+        <v>3018</v>
+      </c>
+      <c r="B3162" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3162" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3162" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3162" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3163" s="2" t="s">
+        <v>3021</v>
+      </c>
+      <c r="B3163" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3163" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3163" s="5"/>
+      <c r="E3163" s="5" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="3164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3164" s="2" t="s">
+        <v>3021</v>
+      </c>
+      <c r="B3164" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="C3164" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3164" s="5"/>
+      <c r="E3164" s="5" t="s">
+        <v>3022</v>
+      </c>
+    </row>
+    <row r="3165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3165" s="2" t="s">
+        <v>3021</v>
+      </c>
+      <c r="B3165" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="C3165" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3165" s="5"/>
+      <c r="E3165" s="5" t="s">
+        <v>3023</v>
+      </c>
+    </row>
+    <row r="3166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3166" s="2" t="s">
+        <v>3021</v>
+      </c>
+      <c r="B3166" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C3166" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3166" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="E3166" s="5" t="s">
+        <v>3024</v>
+      </c>
+    </row>
+    <row r="3167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3167" s="2" t="s">
+        <v>3021</v>
+      </c>
+      <c r="B3167" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3167" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3167" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="E3167" s="5" t="s">
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="3168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3168" s="2" t="s">
+        <v>3021</v>
+      </c>
+      <c r="B3168" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3168" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3168" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="E3168" s="5" t="s">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="3169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3169" s="2" t="s">
+        <v>3021</v>
+      </c>
+      <c r="B3169" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="C3169" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3169" s="5" t="s">
+        <v>3027</v>
+      </c>
+      <c r="E3169" s="5" t="s">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="3170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3170" s="2" t="s">
+        <v>3021</v>
+      </c>
+      <c r="B3170" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3170" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3170" s="5" t="s">
+        <v>3027</v>
+      </c>
+      <c r="E3170" s="5" t="s">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="3171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3171" s="2" t="s">
+        <v>3021</v>
+      </c>
+      <c r="B3171" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3171" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3171" s="5" t="s">
+        <v>3027</v>
+      </c>
+      <c r="E3171" s="5" t="s">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="3172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3172" s="2" t="s">
+        <v>3029</v>
+      </c>
+      <c r="B3172" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3172" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3172" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3172" s="5" t="s">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="3173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3173" s="2" t="s">
+        <v>3031</v>
+      </c>
+      <c r="B3173" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3173" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3173" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3173" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3174" s="2" t="s">
+        <v>3031</v>
+      </c>
+      <c r="B3174" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3174" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D3174" s="5" t="s">
+        <v>1317</v>
+      </c>
+      <c r="E3174" s="5" t="s">
+        <v>3032</v>
+      </c>
+    </row>
+    <row r="3175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3175" s="6" t="s">
+        <v>3034</v>
+      </c>
+      <c r="B3175" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3175" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3175" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3175" s="7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3176" s="6" t="s">
+        <v>3034</v>
+      </c>
+      <c r="B3176" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3176" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3176" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3176" s="7" t="s">
+        <v>3033</v>
+      </c>
+    </row>
+    <row r="3177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3177" s="6" t="s">
+        <v>3035</v>
+      </c>
+      <c r="B3177" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3177" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3177" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3177" s="7" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="3178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3178" s="6"/>
+      <c r="B3178" s="6"/>
+      <c r="C3178" s="6"/>
+      <c r="D3178" s="6"/>
+      <c r="E3178" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>